<commit_message>
mblack review and update
</commit_message>
<xml_diff>
--- a/release-notes/2024-10/closed-bugs-sle-2024-10.xlsx
+++ b/release-notes/2024-10/closed-bugs-sle-2024-10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nio365.sharepoint.com/sites/IoTProgram/Shared Documents/ProjectDocuments/SystemLink 2024/2024 Q4 (v.24.8)(releasing out of Cycle 24.C3)/Common docs/Release notes/SLE 2024-09 Release Notes - August iteration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/github/install-systemlink-enterprise/release-notes/2024-10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{0357FC32-4DB0-FA47-B55E-60093BEFF741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06E9A9B4-9CF6-47F1-9119-2360135198F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB15505-9876-DE49-AD87-EDFCC13F8DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="22880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed bugs in last iteration" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>[UI] Some asset properties are not shown in the correct format</t>
   </si>
   <si>
-    <t>[GM reported] FeedService.WebAPI - CVE-2021-26701</t>
-  </si>
-  <si>
     <t>WebAppServices helm chart does not set readOnlyRootFilesystem: true</t>
   </si>
   <si>
@@ -183,13 +180,16 @@
   </si>
   <si>
     <t>[States UI] Panel editor not accouting for newly created custom properties</t>
+  </si>
+  <si>
+    <t>FeedService.WebAPI - CVE-2021-26701</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -674,8 +674,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -735,9 +735,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -775,7 +775,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -881,7 +881,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1023,7 +1023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1034,15 +1034,16 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="110.375" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="110.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2851937</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2847881</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2843156</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2845232</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2857332</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2860025</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2869684</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2879581</v>
       </c>
@@ -1141,7 +1142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2879813</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2883234</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2884840</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2863977</v>
       </c>
@@ -1185,364 +1186,364 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2901936</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2855043</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2850466</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2861857</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2858921</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2855124</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2857278</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2854501</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2828594</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2842877</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2843020</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2855098</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2900504</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2870173</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2870174</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2870176</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2835562</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2835700</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2839896</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2840476</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2840913</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2846121</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2859266</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2857864</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2855467</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2855480</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2857692</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2845118</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2845194</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2581683</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2824818</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2866680</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2884878</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -1568,6 +1569,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC68938C25E75A48B38E3943F7278D4C" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d58f385c17140d35cbd71f1f19d1bc6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9" xmlns:ns3="8f35f8fb-94b8-4296-88b5-253c68a5f93d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6fea239938238ce97a7c0b11cdae990" ns2:_="" ns3:_="">
     <xsd:import namespace="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
@@ -1816,23 +1826,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
+    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
+    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating titles for closed bugs
</commit_message>
<xml_diff>
--- a/release-notes/2024-10/closed-bugs-sle-2024-10.xlsx
+++ b/release-notes/2024-10/closed-bugs-sle-2024-10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nio365.sharepoint.com/sites/IoTProgram/Shared Documents/ProjectDocuments/SystemLink 2024/2024 Q4 (v.24.8)(releasing out of Cycle 24.C3)/Common docs/Release notes/SLE 2024-10 Release Notes - September/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/github/install-systemlink-enterprise/release-notes/2024-10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{0357FC32-4DB0-FA47-B55E-60093BEFF741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{529F5081-1BDB-4A39-8734-C85FDB5C9C81}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472D7FDD-0748-BC48-959F-64C598C38AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17730" yWindow="-16200" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25540" yWindow="0" windowWidth="10300" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed bugs in last iteration" sheetId="1" r:id="rId1"/>
@@ -47,21 +47,12 @@
     <t>State</t>
   </si>
   <si>
-    <t>SlUserSelector sometimes resets itself back to current user after being cleared</t>
-  </si>
-  <si>
     <t>Closed</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove inferred bus type value when bus type is not defined in the client </t>
-  </si>
-  <si>
     <t>Update asset fails when either ModelName, Model number, VendorName, VendorNumber are empty</t>
   </si>
   <si>
-    <t>History tab should update query request when changing the current asset</t>
-  </si>
-  <si>
     <t>[Assets UI] Editing calibration info does not work when selecting a different date from the date picker</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>[UI] Some asset properties are not shown in the correct format</t>
   </si>
   <si>
-    <t>[GM reported] FeedService.WebAPI - CVE-2021-26701</t>
-  </si>
-  <si>
     <t>WebAppServices helm chart does not set readOnlyRootFilesystem: true</t>
   </si>
   <si>
@@ -110,15 +98,9 @@
     <t>Untouched DUT control displays error when creating a test plan</t>
   </si>
   <si>
-    <t>Alarm and DFS example continuation tokens are invalid</t>
-  </si>
-  <si>
     <t>500 error when continuationToken is an empty string for /nialarm/v1/query-instances-with-filter</t>
   </si>
   <si>
-    <t>RBAC integrator doesn't emit the duration metric when the job fails</t>
-  </si>
-  <si>
     <t>Grafana container does not set readOnlyRootFilesystem: true</t>
   </si>
   <si>
@@ -182,7 +164,25 @@
     <t>[States UI] Panel editor not accouting for newly created custom properties</t>
   </si>
   <si>
-    <t>Unable to download large files from the Files grid</t>
+    <t>"Assigned to" user selector in Test Plans sometimes resets itself back to current user after being cleared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove inferred bus type value for an asset when bus type is not defined in the client </t>
+  </si>
+  <si>
+    <t>Asset Location tab should update query request when changing the current asset</t>
+  </si>
+  <si>
+    <t>FeedService.WebAPI - CVE-2021-26701</t>
+  </si>
+  <si>
+    <t>Alarm and DFS example continuation tokens in Swagger UI are invalid</t>
+  </si>
+  <si>
+    <t>RBAC integrator container doesn't emit the duration metric when the job fails</t>
+  </si>
+  <si>
+    <t>Users can't download files larger than 10MB from the files grid</t>
   </si>
 </sst>
 </file>
@@ -1033,16 +1033,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="110.34765625" customWidth="1"/>
+    <col min="2" max="2" width="110.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1053,458 +1053,458 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2851937</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2847881</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2843156</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2845232</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2857332</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2860025</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2869684</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2879581</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2879813</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2883234</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2884840</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2863977</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2901936</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2855043</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2850466</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2861857</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2858921</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2855124</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2857278</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2854501</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2828594</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2842877</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2843020</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2855098</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2900504</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2870173</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2870174</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2870176</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2835562</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2835700</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2839896</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2840476</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2840913</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2846121</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2859266</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2857864</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2855467</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2855480</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2857692</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2845118</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2845194</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2581683</v>
       </c>
@@ -1512,40 +1512,40 @@
         <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2824818</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2866680</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2884878</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1568,15 +1568,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC68938C25E75A48B38E3943F7278D4C" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d58f385c17140d35cbd71f1f19d1bc6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9" xmlns:ns3="8f35f8fb-94b8-4296-88b5-253c68a5f93d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6fea239938238ce97a7c0b11cdae990" ns2:_="" ns3:_="">
     <xsd:import namespace="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
@@ -1825,6 +1816,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
   <ds:schemaRefs>
@@ -1843,14 +1843,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1867,4 +1859,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>